<commit_message>
transformed graphs into a more fitting format
</commit_message>
<xml_diff>
--- a/presentation/data/all.xlsx
+++ b/presentation/data/all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tinnyx\Dropbox\work\PV254-recommender-system\presentation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A84D11-1DE9-43EE-93A3-0BA8A95B07B0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B197A113-CC69-4B4E-9778-5869342ABF4A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11970" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -19827,8 +19827,8 @@
       <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
@@ -19904,7 +19904,7 @@
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -19981,8 +19981,8 @@
       <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>561976</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
@@ -20058,8 +20058,8 @@
       <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
@@ -20135,7 +20135,7 @@
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -20465,7 +20465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3918"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -71042,8 +71042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R45" sqref="R45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>